<commit_message>
backup for latex writing and some minor model fixes
</commit_message>
<xml_diff>
--- a/gams/res_sum_Q_in_RL.xlsx
+++ b/gams/res_sum_Q_in_RL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\CloudDrive\Uni\WS24\Research Project\gams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5896D87-35B9-4DFC-A3B3-01B68070EFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E47EEAD-1581-4542-B76B-82522C7A0EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="795" windowWidth="16440" windowHeight="28440" xr2:uid="{ADE2AEB3-5F5D-46E2-9874-D3B5C27C0EB5}"/>
+    <workbookView xWindow="-9690" yWindow="990" windowWidth="7500" windowHeight="6000" xr2:uid="{ADE2AEB3-5F5D-46E2-9874-D3B5C27C0EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
backup before the s_RA reformulation
because s_RA doesnt represent prices to choose anymore but different scenarios on the next day that could happen i need to reformulate some equations ... this is the backup before reformulation

not 100% if i already reformulated 1 or 2 equations
</commit_message>
<xml_diff>
--- a/gams/res_sum_Q_in_RL.xlsx
+++ b/gams/res_sum_Q_in_RL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\CloudDrive\Uni\WS24\Research Project\gams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E47EEAD-1581-4542-B76B-82522C7A0EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F491D79C-7766-4CFB-83FE-7328B6D28D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9690" yWindow="990" windowWidth="7500" windowHeight="6000" xr2:uid="{ADE2AEB3-5F5D-46E2-9874-D3B5C27C0EB5}"/>
+    <workbookView xWindow="-16320" yWindow="795" windowWidth="16440" windowHeight="28440" xr2:uid="{ADE2AEB3-5F5D-46E2-9874-D3B5C27C0EB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>4.5</v>
+        <v>2.8728000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>